<commit_message>
Fixing PS table for Andrew's rate studies
</commit_message>
<xml_diff>
--- a/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-RateStudyAndrew.xlsx
+++ b/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-RateStudyAndrew.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02C31F-179B-AA44-90F9-0F74923059EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049F84B-468E-684B-B444-4C76204C876D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-420" yWindow="-19300" windowWidth="28620" windowHeight="16720" xr2:uid="{D43503D0-D942-054C-A252-8EF60B2ECDE6}"/>
   </bookViews>
@@ -1459,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46014C27-F11A-2A41-BE5F-BBB4784EB01D}">
   <dimension ref="A1:E344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="E303" sqref="E303"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3623,8 +3623,8 @@
       <c r="D127" s="1">
         <v>1</v>
       </c>
-      <c r="E127" s="1">
-        <v>1</v>
+      <c r="E127" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3980,8 +3980,8 @@
       <c r="D148" s="1">
         <v>1</v>
       </c>
-      <c r="E148" s="1">
-        <v>1</v>
+      <c r="E148" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -4014,8 +4014,8 @@
       <c r="D150" s="1">
         <v>1</v>
       </c>
-      <c r="E150" s="1">
-        <v>1</v>
+      <c r="E150" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -6326,8 +6326,8 @@
       <c r="D286" s="1">
         <v>1</v>
       </c>
-      <c r="E286" s="1">
-        <v>1</v>
+      <c r="E286" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
@@ -7318,5 +7318,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>